<commit_message>
line and link opening editing
</commit_message>
<xml_diff>
--- a/Output/output_with_messages.xlsx
+++ b/Output/output_with_messages.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -55,10 +55,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,79 +431,94 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="24" customWidth="1" min="1" max="1"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="3" max="3"/>
+    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="21" customWidth="1" min="6" max="6"/>
+    <col width="30" customWidth="1" min="7" max="7"/>
+    <col width="30" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Business Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Owner/Manager</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Phone Number</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>DISPOSITION</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>WittyMessage</t>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Message</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Event</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>Mary Davis Cable</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Mary Davis</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>(973) 489-8596</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr"/>
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>405 Tennessee AveAthens, TN 37303</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <t>WN</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="3" t="inlineStr">
         <is>
           <t>Hi Mary Davis,
 🎉 Congratulations on taking the first step towards an even brighter future for Mary Davis Cable! 🎉
@@ -508,35 +529,40 @@
 Blabor Team</t>
         </is>
       </c>
+      <c r="H2" s="3" t="inlineStr">
+        <is>
+          <t>Link click tracked for Mary Davis Cable: opened</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>Milestone Chiropractic</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Wyatt Campbell</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>(973) 489-8596</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr"/>
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>611 N Maple StMurfreesboro, TN 37130</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
         <is>
           <t>LM</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="3" t="inlineStr">
         <is>
           <t>Hi Wyatt Campbell,
 🎉 Congratulations on taking the first step towards an even brighter future for Milestone Chiropractic! 🎉
@@ -547,35 +573,40 @@
 Blabor Team</t>
         </is>
       </c>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>Link click tracked for Milestone Chiropractic: opened</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Morehead Demolition</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Teresa Long</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>(201) 492-8580</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr"/>
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>4320 Ringgold RdEast Ridge, TN 37412</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>LM available domain</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="3" t="inlineStr">
         <is>
           <t>Hi Teresa Long,
 🎉 Congratulations on taking the first step towards an even brighter future for Morehead Demolition! 🎉
@@ -586,31 +617,36 @@
 Blabor Team</t>
         </is>
       </c>
+      <c r="H4" s="3" t="inlineStr">
+        <is>
+          <t>Link click tracked for Morehead Demolition: opened</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Motor King LLC</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Alex Pena</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>(657) 799-8283</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr"/>
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>245 S Shadowbay BlvdLuttrell, TN 37779</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr"/>
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>Hi Alex Pena,
 🎉 Congratulations on taking the first step towards an even brighter future for Motor King LLC! 🎉
@@ -621,6 +657,11 @@
 Blabor Team</t>
         </is>
       </c>
+      <c r="H5" s="3" t="inlineStr">
+        <is>
+          <t>Link click tracked for Motor King LLC: opened</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>